<commit_message>
Added Excel files demonstrating absolute/mixed references and conditional logic
</commit_message>
<xml_diff>
--- a/Formulas and Functions/1_Formulas_Intro.xlsx
+++ b/Formulas and Functions/1_Formulas_Intro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lee\Desktop\Excel\Excel_Data_Analytics_Project\Formulas and Functions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CADC1ED-BA44-427C-BBA1-8958712DD411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC0F7E02-843F-41B5-9B75-881541F27A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8CC555B5-3E06-43B6-9E5B-C0A1D3498DA4}"/>
   </bookViews>
@@ -806,7 +806,7 @@
   <dimension ref="B1:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -816,9 +816,9 @@
     <col min="3" max="3" width="10.44140625" style="4" customWidth="1"/>
     <col min="4" max="4" width="12.21875" style="4" customWidth="1"/>
     <col min="5" max="5" width="11.5546875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="10" style="4" customWidth="1"/>
-    <col min="7" max="13" width="9" style="4"/>
-    <col min="14" max="14" width="11.21875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="10" style="4" hidden="1" customWidth="1"/>
+    <col min="7" max="13" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="11.21875" style="4" hidden="1" customWidth="1"/>
     <col min="15" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
@@ -904,6 +904,22 @@
         <f>E3&gt;D3</f>
         <v>0</v>
       </c>
+      <c r="L3" s="4" t="b">
+        <f>$C$15&lt;=C3</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="4" t="b">
+        <f>$G3&gt;=C$16</f>
+        <v>1</v>
+      </c>
+      <c r="N3" s="4">
+        <f>L3*M3</f>
+        <v>0</v>
+      </c>
+      <c r="O3" s="4" t="b">
+        <f>N3=1</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
@@ -942,6 +958,22 @@
         <f t="shared" ref="K4:K12" si="5">E4&gt;D4</f>
         <v>0</v>
       </c>
+      <c r="L4" s="4" t="b">
+        <f t="shared" ref="L4:L12" si="6">$C$15&lt;=C4</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="4" t="b">
+        <f t="shared" ref="M3:M11" si="7">$G4&gt;=C$16</f>
+        <v>1</v>
+      </c>
+      <c r="N4" s="4">
+        <f t="shared" ref="N4:N12" si="8">L4*M4</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="4" t="b">
+        <f t="shared" ref="O4:O12" si="9">N4=1</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
@@ -980,6 +1012,22 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
+      <c r="L5" s="4" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M5" s="4" t="b">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N5" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O5" s="4" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
@@ -1018,6 +1066,22 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
+      <c r="L6" s="4" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M6" s="4" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N6" s="4">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="O6" s="4" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B7" s="8" t="s">
@@ -1056,6 +1120,22 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
+      <c r="L7" s="4" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M7" s="4" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N7" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O7" s="4" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B8" s="8" t="s">
@@ -1094,6 +1174,22 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
+      <c r="L8" s="4" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M8" s="4" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N8" s="4">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="O8" s="4" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B9" s="8" t="s">
@@ -1132,6 +1228,22 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
+      <c r="L9" s="4" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M9" s="4" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N9" s="4">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="O9" s="4" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B10" s="8" t="s">
@@ -1170,6 +1282,22 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
+      <c r="L10" s="4" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M10" s="4" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N10" s="4">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="O10" s="4" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B11" s="8" t="s">
@@ -1208,6 +1336,22 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
+      <c r="L11" s="4" t="b">
+        <f>$C$15&lt;=C11</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="4" t="b">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="N11" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="4" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="11" t="s">
@@ -1246,6 +1390,22 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
+      <c r="L12" s="4" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="4" t="b">
+        <f>$G12&gt;=C$16</f>
+        <v>1</v>
+      </c>
+      <c r="N12" s="4">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O12" s="4" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="29" t="s">
@@ -1256,13 +1416,17 @@
       <c r="B15" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="26"/>
+      <c r="C15" s="26">
+        <v>6</v>
+      </c>
     </row>
     <row r="16" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="28"/>
+      <c r="C16" s="28">
+        <v>90000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Checked on Logical functions and formulas,
</commit_message>
<xml_diff>
--- a/Formulas and Functions/1_Formulas_Intro.xlsx
+++ b/Formulas and Functions/1_Formulas_Intro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lee\Desktop\Excel\Excel_Data_Analytics_Project\Formulas and Functions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC0F7E02-843F-41B5-9B75-881541F27A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DBA0ECF-B884-4AE7-B8F2-79CA89A0DE7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8CC555B5-3E06-43B6-9E5B-C0A1D3498DA4}"/>
   </bookViews>
@@ -803,10 +803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95A41B6C-80F1-4D7E-AD46-00EDEBFEC87C}">
-  <dimension ref="B1:O16"/>
+  <dimension ref="B1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -817,13 +817,15 @@
     <col min="4" max="4" width="12.21875" style="4" customWidth="1"/>
     <col min="5" max="5" width="11.5546875" style="4" customWidth="1"/>
     <col min="6" max="6" width="10" style="4" hidden="1" customWidth="1"/>
-    <col min="7" max="13" width="0" style="4" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="11.21875" style="4" hidden="1" customWidth="1"/>
+    <col min="7" max="11" width="0" style="4" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="9" style="4" customWidth="1"/>
+    <col min="13" max="13" width="11.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.5546875" style="4" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
         <v>10</v>
       </c>
@@ -867,7 +869,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
         <v>0</v>
       </c>
@@ -920,8 +922,12 @@
         <f>N3=1</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P3" s="4" t="str">
+        <f>IF(M3,"Goal Met","Not Met")</f>
+        <v>Goal Met</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
@@ -974,8 +980,12 @@
         <f t="shared" ref="O4:O12" si="9">N4=1</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P4" s="4" t="str">
+        <f t="shared" ref="P4:P12" si="10">IF(M4,"Goal Met","Not Met")</f>
+        <v>Goal Met</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
         <v>2</v>
       </c>
@@ -1028,8 +1038,12 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P5" s="4" t="str">
+        <f t="shared" si="10"/>
+        <v>Not Met</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
         <v>3</v>
       </c>
@@ -1082,8 +1096,12 @@
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P6" s="4" t="str">
+        <f t="shared" si="10"/>
+        <v>Goal Met</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" s="8" t="s">
         <v>4</v>
       </c>
@@ -1136,8 +1154,12 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P7" s="4" t="str">
+        <f t="shared" si="10"/>
+        <v>Goal Met</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8" s="8" t="s">
         <v>5</v>
       </c>
@@ -1190,8 +1212,12 @@
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P8" s="4" t="str">
+        <f t="shared" si="10"/>
+        <v>Goal Met</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" s="8" t="s">
         <v>6</v>
       </c>
@@ -1244,8 +1270,12 @@
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P9" s="4" t="str">
+        <f t="shared" si="10"/>
+        <v>Goal Met</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" s="8" t="s">
         <v>7</v>
       </c>
@@ -1298,8 +1328,12 @@
         <f t="shared" si="9"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P10" s="4" t="str">
+        <f t="shared" si="10"/>
+        <v>Goal Met</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B11" s="8" t="s">
         <v>8</v>
       </c>
@@ -1352,8 +1386,12 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P11" s="4" t="str">
+        <f t="shared" si="10"/>
+        <v>Goal Met</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="11" t="s">
         <v>9</v>
       </c>
@@ -1406,13 +1444,17 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P12" s="4" t="str">
+        <f t="shared" si="10"/>
+        <v>Goal Met</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="29" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B15" s="25" t="s">
         <v>48</v>
       </c>
@@ -1420,7 +1462,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="27" t="s">
         <v>49</v>
       </c>

</xml_diff>